<commit_message>
init frint calc math 5
</commit_message>
<xml_diff>
--- a/Вычмат/lab5/вычя.xlsx
+++ b/Вычмат/lab5/вычя.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\docs_for_labs\Вычмат\lab5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs_for_labs\docs_for_labs\Вычмат\lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6702F2AB-76A9-40EA-8886-C0726D545E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>x1*</t>
   </si>
   <si>
@@ -68,9 +64,6 @@
     <t>dy6</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -84,12 +77,18 @@
   </si>
   <si>
     <t>(x-1,1)/0,15</t>
+  </si>
+  <si>
+    <t>dy0</t>
+  </si>
+  <si>
+    <t>t_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -108,12 +107,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,9 +133,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -410,85 +421,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B1" sqref="B1:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0.22339999999999999</v>
       </c>
-      <c r="C2">
-        <f>B3-B2</f>
+      <c r="C2" s="2">
+        <f t="shared" ref="C2:H2" si="0">B3-B2</f>
         <v>1.0204</v>
       </c>
-      <c r="D2">
-        <f>C3-C2</f>
+      <c r="D2" s="2">
+        <f t="shared" si="0"/>
         <v>2.0000000000020002E-4</v>
       </c>
-      <c r="E2">
-        <f>D3-D2</f>
+      <c r="E2" s="2">
+        <f t="shared" si="0"/>
         <v>1.3199999999999434E-2</v>
       </c>
-      <c r="F2">
-        <f>E3-E2</f>
+      <c r="F2" s="2">
+        <f t="shared" si="0"/>
         <v>-3.6799999999999278E-2</v>
       </c>
-      <c r="G2">
-        <f>F3-F2</f>
+      <c r="G2" s="3">
+        <f t="shared" si="0"/>
         <v>7.620000000000049E-2</v>
       </c>
-      <c r="H2">
-        <f>G3-G2</f>
+      <c r="H2" s="3">
+        <f t="shared" si="0"/>
         <v>-0.13130000000000508</v>
       </c>
       <c r="J2">
@@ -498,57 +509,60 @@
         <v>1.482</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.25</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>1.2438</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:F8" si="0">B4-B3</f>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:F7" si="1">B4-B3</f>
         <v>1.0206000000000002</v>
       </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
+      <c r="D3" s="2">
+        <f t="shared" si="1"/>
         <v>1.3399999999999634E-2</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
+      <c r="E3" s="3">
+        <f t="shared" si="1"/>
         <v>-2.3599999999999843E-2</v>
       </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
+      <c r="F3" s="3">
+        <f t="shared" si="1"/>
         <v>3.9400000000001212E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <f>F4-F3</f>
         <v>-5.510000000000459E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2.2644000000000002</v>
       </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
+      <c r="C4" s="3">
+        <f t="shared" si="1"/>
         <v>1.0339999999999998</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
+      <c r="D4" s="3">
+        <f t="shared" si="1"/>
         <v>-1.0200000000000209E-2</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
         <v>1.5800000000001369E-2</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
+      <c r="F4" s="2">
+        <f t="shared" si="1"/>
         <v>-1.5700000000003378E-2</v>
       </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
       <c r="J4" t="s">
         <v>10</v>
       </c>
@@ -557,75 +571,100 @@
         <v>0.14999999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.55</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>3.2984</v>
       </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
+      <c r="C5" s="2">
+        <f t="shared" si="1"/>
         <v>1.0237999999999996</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
         <v>5.6000000000011596E-3</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
         <v>9.9999999997990585E-5</v>
       </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
       <c r="J5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1.7</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>4.3221999999999996</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
+      <c r="C6" s="2">
+        <f t="shared" si="1"/>
         <v>1.0294000000000008</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
         <v>5.6999999999991502E-3</v>
       </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1.85</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>5.3516000000000004</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
+      <c r="C7" s="2">
+        <f t="shared" si="1"/>
         <v>1.0350999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>6.3867000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8">
+        <f>(K2-A5)/K4</f>
+        <v>-0.45333333333333403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>0</v>
       </c>
@@ -648,9 +687,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <f>B2</f>
@@ -661,27 +700,27 @@
         <v>1.0204</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:H12" si="1">D2</f>
+        <f t="shared" ref="D12:H12" si="2">D2</f>
         <v>2.0000000000020002E-4</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3199999999999434E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.6799999999999278E-2</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.620000000000049E-2</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.13130000000000508</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>

</xml_diff>